<commit_message>
Long time no see
</commit_message>
<xml_diff>
--- a/NC_filling_estimation/test_matrix_basis.xlsx
+++ b/NC_filling_estimation/test_matrix_basis.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PSI backup\PC9074 office\Data\Data_analysis\NC_filling_estimation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DE97D069-C90D-4F1B-A8C5-3AE11290968F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="17640" windowHeight="10575"/>
+    <workbookView xWindow="1380" yWindow="135" windowWidth="17640" windowHeight="10575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix v2" sheetId="4" r:id="rId1"/>
@@ -12,7 +18,7 @@
     <sheet name="NC calc" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -436,7 +442,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1025,6 +1031,102 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1051,102 +1153,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1160,6 +1166,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1208,7 +1217,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1241,9 +1250,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1276,6 +1302,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1451,11 +1494,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,14 +1583,14 @@
       <c r="D4" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="188" t="s">
+      <c r="E4" s="153" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="188"/>
-      <c r="G4" s="188" t="s">
+      <c r="F4" s="153"/>
+      <c r="G4" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="H4" s="188"/>
+      <c r="H4" s="153"/>
       <c r="I4" s="137" t="s">
         <v>47</v>
       </c>
@@ -1573,7 +1616,7 @@
       <c r="Z4" s="11"/>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="174" t="s">
+      <c r="A5" s="154" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="80" t="s">
@@ -1614,8 +1657,8 @@
       <c r="Z5" s="11"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="175"/>
-      <c r="B6" s="179" t="s">
+      <c r="A6" s="155"/>
+      <c r="B6" s="159" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="30" t="s">
@@ -1638,7 +1681,7 @@
         <f t="shared" ref="H6:H12" si="2">$F$8*(1-D6)</f>
         <v>1</v>
       </c>
-      <c r="I6" s="180" t="s">
+      <c r="I6" s="160" t="s">
         <v>126</v>
       </c>
       <c r="K6" t="str">
@@ -1651,8 +1694,8 @@
       <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="175"/>
-      <c r="B7" s="179"/>
+      <c r="A7" s="155"/>
+      <c r="B7" s="159"/>
       <c r="C7" s="30" t="s">
         <v>59</v>
       </c>
@@ -1673,7 +1716,7 @@
         <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
-      <c r="I7" s="180"/>
+      <c r="I7" s="160"/>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-ABS-2</v>
@@ -1684,8 +1727,8 @@
       <c r="M7" s="11"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="175"/>
-      <c r="B8" s="179"/>
+      <c r="A8" s="155"/>
+      <c r="B8" s="159"/>
       <c r="C8" s="30" t="s">
         <v>60</v>
       </c>
@@ -1706,7 +1749,7 @@
         <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
-      <c r="I8" s="180"/>
+      <c r="I8" s="160"/>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-ABS-3</v>
@@ -1716,8 +1759,8 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="175"/>
-      <c r="B9" s="179"/>
+      <c r="A9" s="155"/>
+      <c r="B9" s="159"/>
       <c r="C9" s="30" t="s">
         <v>61</v>
       </c>
@@ -1738,7 +1781,7 @@
         <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="I9" s="180"/>
+      <c r="I9" s="160"/>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-ABS-4</v>
@@ -1749,8 +1792,8 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="175"/>
-      <c r="B10" s="179"/>
+      <c r="A10" s="155"/>
+      <c r="B10" s="159"/>
       <c r="C10" s="30" t="s">
         <v>62</v>
       </c>
@@ -1767,7 +1810,7 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="I10" s="180"/>
+      <c r="I10" s="160"/>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-ABS-5</v>
@@ -1777,8 +1820,8 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="175"/>
-      <c r="B11" s="179"/>
+      <c r="A11" s="155"/>
+      <c r="B11" s="159"/>
       <c r="C11" s="30" t="s">
         <v>63</v>
       </c>
@@ -1795,7 +1838,7 @@
         <f t="shared" si="2"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="I11" s="180"/>
+      <c r="I11" s="160"/>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-ABS-6</v>
@@ -1805,8 +1848,8 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="175"/>
-      <c r="B12" s="179"/>
+      <c r="A12" s="155"/>
+      <c r="B12" s="159"/>
       <c r="C12" s="30" t="s">
         <v>64</v>
       </c>
@@ -1823,7 +1866,7 @@
         <f t="shared" si="2"/>
         <v>9.9999999999999978E-2</v>
       </c>
-      <c r="I12" s="180"/>
+      <c r="I12" s="160"/>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-ABS-7</v>
@@ -1833,7 +1876,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="175"/>
+      <c r="A13" s="155"/>
       <c r="B13" s="85" t="s">
         <v>102</v>
       </c>
@@ -1863,8 +1906,8 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="175"/>
-      <c r="B14" s="177" t="s">
+      <c r="A14" s="155"/>
+      <c r="B14" s="157" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="33" t="s">
@@ -1880,14 +1923,14 @@
         <v>20</v>
       </c>
       <c r="G14" s="36">
-        <f t="shared" ref="G14:G20" si="3">$F$16/(1-D14)</f>
-        <v>1</v>
+        <f>$F$16/(1-D14)*$F$17</f>
+        <v>2</v>
       </c>
       <c r="H14" s="35">
         <f>1-$F$16/G14</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="181" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="161" t="s">
         <v>126</v>
       </c>
       <c r="K14" t="str">
@@ -1899,8 +1942,8 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="175"/>
-      <c r="B15" s="177"/>
+      <c r="A15" s="155"/>
+      <c r="B15" s="157"/>
       <c r="C15" s="33" t="s">
         <v>66</v>
       </c>
@@ -1914,14 +1957,14 @@
         <v>1</v>
       </c>
       <c r="G15" s="36">
-        <f t="shared" si="3"/>
-        <v>1.1111111111111112</v>
+        <f t="shared" ref="G15:G18" si="3">$F$16/(1-D15)*$F$17</f>
+        <v>2.2222222222222223</v>
       </c>
       <c r="H15" s="35">
         <f t="shared" ref="H15:H20" si="4">1-$F$16/G15</f>
-        <v>0.10000000000000009</v>
-      </c>
-      <c r="I15" s="181"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I15" s="161"/>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-PART-2</v>
@@ -1931,8 +1974,8 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="175"/>
-      <c r="B16" s="177"/>
+      <c r="A16" s="155"/>
+      <c r="B16" s="157"/>
       <c r="C16" s="33" t="s">
         <v>67</v>
       </c>
@@ -1947,13 +1990,13 @@
       </c>
       <c r="G16" s="36">
         <f t="shared" si="3"/>
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="H16" s="35">
         <f t="shared" si="4"/>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="I16" s="181"/>
+        <v>0.6</v>
+      </c>
+      <c r="I16" s="161"/>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-PART-3</v>
@@ -1963,8 +2006,8 @@
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="175"/>
-      <c r="B17" s="177"/>
+      <c r="A17" s="155"/>
+      <c r="B17" s="157"/>
       <c r="C17" s="33" t="s">
         <v>68</v>
       </c>
@@ -1979,13 +2022,13 @@
       </c>
       <c r="G17" s="36">
         <f t="shared" si="3"/>
-        <v>1.4285714285714286</v>
+        <v>2.8571428571428572</v>
       </c>
       <c r="H17" s="35">
         <f t="shared" si="4"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="I17" s="181"/>
+        <v>0.65</v>
+      </c>
+      <c r="I17" s="161"/>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-PART-4</v>
@@ -1996,8 +2039,8 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" s="175"/>
-      <c r="B18" s="177"/>
+      <c r="A18" s="155"/>
+      <c r="B18" s="157"/>
       <c r="C18" s="33" t="s">
         <v>69</v>
       </c>
@@ -2008,13 +2051,13 @@
       <c r="F18" s="35"/>
       <c r="G18" s="36">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H18" s="35">
         <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="I18" s="181"/>
+        <v>0.75</v>
+      </c>
+      <c r="I18" s="161"/>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-PART-5</v>
@@ -2024,8 +2067,8 @@
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A19" s="175"/>
-      <c r="B19" s="177"/>
+      <c r="A19" s="155"/>
+      <c r="B19" s="157"/>
       <c r="C19" s="33" t="s">
         <v>70</v>
       </c>
@@ -2035,14 +2078,14 @@
       <c r="E19" s="35"/>
       <c r="F19" s="35"/>
       <c r="G19" s="36">
-        <f t="shared" si="3"/>
-        <v>3.333333333333333</v>
+        <f>$F$16/(1-D19)*$F$17</f>
+        <v>6.6666666666666661</v>
       </c>
       <c r="H19" s="35">
         <f t="shared" si="4"/>
-        <v>0.7</v>
-      </c>
-      <c r="I19" s="181"/>
+        <v>0.85</v>
+      </c>
+      <c r="I19" s="161"/>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-PART-6</v>
@@ -2052,8 +2095,8 @@
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A20" s="176"/>
-      <c r="B20" s="178"/>
+      <c r="A20" s="156"/>
+      <c r="B20" s="158"/>
       <c r="C20" s="37" t="s">
         <v>71</v>
       </c>
@@ -2063,14 +2106,14 @@
       <c r="E20" s="39"/>
       <c r="F20" s="39"/>
       <c r="G20" s="40">
-        <f t="shared" si="3"/>
-        <v>5.0000000000000009</v>
+        <f>$F$16/(1-D20)*$F$17</f>
+        <v>10.000000000000002</v>
       </c>
       <c r="H20" s="35">
         <f t="shared" si="4"/>
-        <v>0.8</v>
-      </c>
-      <c r="I20" s="182"/>
+        <v>0.9</v>
+      </c>
+      <c r="I20" s="162"/>
       <c r="K20" t="str">
         <f t="shared" si="0"/>
         <v>NC-MFR-PART-7</v>
@@ -2080,7 +2123,7 @@
       </c>
     </row>
     <row r="21" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="171" t="s">
+      <c r="A21" s="170" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="91" t="s">
@@ -2112,8 +2155,8 @@
       </c>
     </row>
     <row r="22" spans="1:32" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="172"/>
-      <c r="B22" s="158" t="s">
+      <c r="A22" s="171"/>
+      <c r="B22" s="174" t="s">
         <v>56</v>
       </c>
       <c r="C22" s="41" t="s">
@@ -2133,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="43"/>
-      <c r="I22" s="183" t="s">
+      <c r="I22" s="148" t="s">
         <v>48</v>
       </c>
       <c r="K22" t="str">
@@ -2145,8 +2188,8 @@
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A23" s="172"/>
-      <c r="B23" s="158"/>
+      <c r="A23" s="171"/>
+      <c r="B23" s="174"/>
       <c r="C23" s="41" t="s">
         <v>73</v>
       </c>
@@ -2164,7 +2207,7 @@
         <v>0.69986342165326432</v>
       </c>
       <c r="H23" s="43"/>
-      <c r="I23" s="183"/>
+      <c r="I23" s="148"/>
       <c r="K23" t="str">
         <f t="shared" si="0"/>
         <v>NC-CMP-2</v>
@@ -2174,8 +2217,8 @@
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A24" s="172"/>
-      <c r="B24" s="158"/>
+      <c r="A24" s="171"/>
+      <c r="B24" s="174"/>
       <c r="C24" s="41" t="s">
         <v>74</v>
       </c>
@@ -2193,7 +2236,7 @@
         <v>0.87492885734728687</v>
       </c>
       <c r="H24" s="43"/>
-      <c r="I24" s="183"/>
+      <c r="I24" s="148"/>
       <c r="K24" t="str">
         <f t="shared" si="0"/>
         <v>NC-CMP-3</v>
@@ -2203,8 +2246,8 @@
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A25" s="172"/>
-      <c r="B25" s="158"/>
+      <c r="A25" s="171"/>
+      <c r="B25" s="174"/>
       <c r="C25" s="41" t="s">
         <v>75</v>
       </c>
@@ -2222,7 +2265,7 @@
         <v>0.95451723120641374</v>
       </c>
       <c r="H25" s="43"/>
-      <c r="I25" s="183"/>
+      <c r="I25" s="148"/>
       <c r="K25" t="str">
         <f t="shared" si="0"/>
         <v>NC-CMP-4</v>
@@ -2232,8 +2275,8 @@
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A26" s="173"/>
-      <c r="B26" s="159"/>
+      <c r="A26" s="172"/>
+      <c r="B26" s="175"/>
       <c r="C26" s="45" t="s">
         <v>76</v>
       </c>
@@ -2252,7 +2295,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="47"/>
-      <c r="I26" s="184"/>
+      <c r="I26" s="149"/>
       <c r="K26" t="str">
         <f t="shared" si="0"/>
         <v>NC-CMP-5</v>
@@ -2263,7 +2306,7 @@
       <c r="AF26" s="11"/>
     </row>
     <row r="27" spans="1:32" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="185" t="s">
+      <c r="A27" s="150" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="97" t="s">
@@ -2293,8 +2336,8 @@
       </c>
     </row>
     <row r="28" spans="1:32" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="186"/>
-      <c r="B28" s="157" t="s">
+      <c r="A28" s="151"/>
+      <c r="B28" s="173" t="s">
         <v>42</v>
       </c>
       <c r="C28" s="49" t="s">
@@ -2314,7 +2357,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="50"/>
-      <c r="I28" s="148" t="s">
+      <c r="I28" s="180" t="s">
         <v>48</v>
       </c>
       <c r="K28" t="str">
@@ -2326,8 +2369,8 @@
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A29" s="186"/>
-      <c r="B29" s="157"/>
+      <c r="A29" s="151"/>
+      <c r="B29" s="173"/>
       <c r="C29" s="49" t="s">
         <v>117</v>
       </c>
@@ -2345,7 +2388,7 @@
         <v>2</v>
       </c>
       <c r="H29" s="50"/>
-      <c r="I29" s="148"/>
+      <c r="I29" s="180"/>
       <c r="K29" t="str">
         <f t="shared" si="0"/>
         <v>Pabs-MFR-2</v>
@@ -2355,8 +2398,8 @@
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A30" s="186"/>
-      <c r="B30" s="157"/>
+      <c r="A30" s="151"/>
+      <c r="B30" s="173"/>
       <c r="C30" s="49" t="s">
         <v>118</v>
       </c>
@@ -2374,7 +2417,7 @@
         <v>3</v>
       </c>
       <c r="H30" s="50"/>
-      <c r="I30" s="148"/>
+      <c r="I30" s="180"/>
       <c r="K30" t="str">
         <f t="shared" si="0"/>
         <v>Pabs-MFR-3</v>
@@ -2384,8 +2427,8 @@
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A31" s="186"/>
-      <c r="B31" s="157"/>
+      <c r="A31" s="151"/>
+      <c r="B31" s="173"/>
       <c r="C31" s="49" t="s">
         <v>119</v>
       </c>
@@ -2403,7 +2446,7 @@
         <v>4</v>
       </c>
       <c r="H31" s="50"/>
-      <c r="I31" s="148"/>
+      <c r="I31" s="180"/>
       <c r="K31" t="str">
         <f t="shared" si="0"/>
         <v>Pabs-MFR-4</v>
@@ -2413,8 +2456,8 @@
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="186"/>
-      <c r="B32" s="157"/>
+      <c r="A32" s="151"/>
+      <c r="B32" s="173"/>
       <c r="C32" s="49" t="s">
         <v>120</v>
       </c>
@@ -2428,7 +2471,7 @@
         <v>5</v>
       </c>
       <c r="H32" s="50"/>
-      <c r="I32" s="148"/>
+      <c r="I32" s="180"/>
       <c r="K32" t="str">
         <f t="shared" si="0"/>
         <v>Pabs-MFR-5</v>
@@ -2438,7 +2481,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="186"/>
+      <c r="A33" s="151"/>
       <c r="B33" s="102" t="s">
         <v>102</v>
       </c>
@@ -2466,8 +2509,8 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="186"/>
-      <c r="B34" s="160" t="s">
+      <c r="A34" s="151"/>
+      <c r="B34" s="176" t="s">
         <v>106</v>
       </c>
       <c r="C34" s="52" t="s">
@@ -2487,7 +2530,7 @@
         <v>0.5</v>
       </c>
       <c r="H34" s="53"/>
-      <c r="I34" s="156" t="s">
+      <c r="I34" s="188" t="s">
         <v>48</v>
       </c>
       <c r="K34" t="str">
@@ -2499,8 +2542,8 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="186"/>
-      <c r="B35" s="160"/>
+      <c r="A35" s="151"/>
+      <c r="B35" s="176"/>
       <c r="C35" s="52" t="s">
         <v>122</v>
       </c>
@@ -2518,7 +2561,7 @@
         <v>0.75</v>
       </c>
       <c r="H35" s="53"/>
-      <c r="I35" s="156"/>
+      <c r="I35" s="188"/>
       <c r="K35" t="str">
         <f t="shared" si="0"/>
         <v>Pabs-PART-2</v>
@@ -2528,8 +2571,8 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="186"/>
-      <c r="B36" s="160"/>
+      <c r="A36" s="151"/>
+      <c r="B36" s="176"/>
       <c r="C36" s="52" t="s">
         <v>123</v>
       </c>
@@ -2547,7 +2590,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="H36" s="53"/>
-      <c r="I36" s="156"/>
+      <c r="I36" s="188"/>
       <c r="K36" t="str">
         <f t="shared" si="0"/>
         <v>Pabs-PART-3</v>
@@ -2557,8 +2600,8 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="186"/>
-      <c r="B37" s="160"/>
+      <c r="A37" s="151"/>
+      <c r="B37" s="176"/>
       <c r="C37" s="52" t="s">
         <v>124</v>
       </c>
@@ -2576,7 +2619,7 @@
         <v>0.875</v>
       </c>
       <c r="H37" s="53"/>
-      <c r="I37" s="156"/>
+      <c r="I37" s="188"/>
       <c r="K37" t="str">
         <f t="shared" ref="K37:K69" si="6">C37</f>
         <v>Pabs-PART-4</v>
@@ -2586,8 +2629,8 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="186"/>
-      <c r="B38" s="160"/>
+      <c r="A38" s="151"/>
+      <c r="B38" s="176"/>
       <c r="C38" s="52" t="s">
         <v>125</v>
       </c>
@@ -2601,7 +2644,7 @@
         <v>0.9</v>
       </c>
       <c r="H38" s="53"/>
-      <c r="I38" s="156"/>
+      <c r="I38" s="188"/>
       <c r="K38" t="str">
         <f t="shared" si="6"/>
         <v>Pabs-PART-5</v>
@@ -2611,7 +2654,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="186"/>
+      <c r="A39" s="151"/>
       <c r="B39" s="108" t="s">
         <v>102</v>
       </c>
@@ -2637,8 +2680,8 @@
       </c>
     </row>
     <row r="40" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="186"/>
-      <c r="B40" s="161" t="s">
+      <c r="A40" s="151"/>
+      <c r="B40" s="177" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="56" t="s">
@@ -2655,7 +2698,7 @@
       </c>
       <c r="G40" s="58"/>
       <c r="H40" s="57"/>
-      <c r="I40" s="154" t="s">
+      <c r="I40" s="186" t="s">
         <v>48</v>
       </c>
       <c r="K40" t="str">
@@ -2667,8 +2710,8 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="186"/>
-      <c r="B41" s="161"/>
+      <c r="A41" s="151"/>
+      <c r="B41" s="177"/>
       <c r="C41" s="56" t="s">
         <v>130</v>
       </c>
@@ -2683,7 +2726,7 @@
       </c>
       <c r="G41" s="58"/>
       <c r="H41" s="57"/>
-      <c r="I41" s="154"/>
+      <c r="I41" s="186"/>
       <c r="K41" t="str">
         <f t="shared" si="6"/>
         <v>Pabs-PURE-2</v>
@@ -2693,8 +2736,8 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="186"/>
-      <c r="B42" s="161"/>
+      <c r="A42" s="151"/>
+      <c r="B42" s="177"/>
       <c r="C42" s="56" t="s">
         <v>131</v>
       </c>
@@ -2709,7 +2752,7 @@
       </c>
       <c r="G42" s="58"/>
       <c r="H42" s="57"/>
-      <c r="I42" s="154"/>
+      <c r="I42" s="186"/>
       <c r="K42" t="str">
         <f t="shared" si="6"/>
         <v>Pabs-PURE-3</v>
@@ -2719,8 +2762,8 @@
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="186"/>
-      <c r="B43" s="161"/>
+      <c r="A43" s="151"/>
+      <c r="B43" s="177"/>
       <c r="C43" s="56" t="s">
         <v>132</v>
       </c>
@@ -2735,7 +2778,7 @@
       </c>
       <c r="G43" s="58"/>
       <c r="H43" s="57"/>
-      <c r="I43" s="154"/>
+      <c r="I43" s="186"/>
       <c r="K43" t="str">
         <f t="shared" si="6"/>
         <v>Pabs-PURE-4</v>
@@ -2745,8 +2788,8 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="187"/>
-      <c r="B44" s="162"/>
+      <c r="A44" s="152"/>
+      <c r="B44" s="178"/>
       <c r="C44" s="56" t="s">
         <v>133</v>
       </c>
@@ -2757,7 +2800,7 @@
       <c r="F44" s="59"/>
       <c r="G44" s="60"/>
       <c r="H44" s="59"/>
-      <c r="I44" s="155"/>
+      <c r="I44" s="187"/>
       <c r="K44" t="str">
         <f t="shared" si="6"/>
         <v>Pabs-PURE-5</v>
@@ -2767,7 +2810,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="164" t="s">
+      <c r="A45" s="163" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="114" t="s">
@@ -2795,8 +2838,8 @@
       </c>
     </row>
     <row r="46" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="165"/>
-      <c r="B46" s="163" t="s">
+      <c r="A46" s="164"/>
+      <c r="B46" s="179" t="s">
         <v>34</v>
       </c>
       <c r="C46" s="61" t="s">
@@ -2813,7 +2856,7 @@
       </c>
       <c r="G46" s="64"/>
       <c r="H46" s="63"/>
-      <c r="I46" s="149" t="s">
+      <c r="I46" s="181" t="s">
         <v>48</v>
       </c>
       <c r="K46" t="str">
@@ -2825,8 +2868,8 @@
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="165"/>
-      <c r="B47" s="163"/>
+      <c r="A47" s="164"/>
+      <c r="B47" s="179"/>
       <c r="C47" s="61" t="s">
         <v>91</v>
       </c>
@@ -2841,7 +2884,7 @@
       </c>
       <c r="G47" s="64"/>
       <c r="H47" s="63"/>
-      <c r="I47" s="149"/>
+      <c r="I47" s="181"/>
       <c r="K47" t="str">
         <f t="shared" si="6"/>
         <v>VEL-DT-NC-2</v>
@@ -2851,8 +2894,8 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="165"/>
-      <c r="B48" s="163"/>
+      <c r="A48" s="164"/>
+      <c r="B48" s="179"/>
       <c r="C48" s="61" t="s">
         <v>92</v>
       </c>
@@ -2867,7 +2910,7 @@
       </c>
       <c r="G48" s="64"/>
       <c r="H48" s="63"/>
-      <c r="I48" s="149"/>
+      <c r="I48" s="181"/>
       <c r="K48" t="str">
         <f t="shared" si="6"/>
         <v>VEL-DT-NC-3</v>
@@ -2877,8 +2920,8 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="165"/>
-      <c r="B49" s="163"/>
+      <c r="A49" s="164"/>
+      <c r="B49" s="179"/>
       <c r="C49" s="61" t="s">
         <v>93</v>
       </c>
@@ -2893,7 +2936,7 @@
       </c>
       <c r="G49" s="64"/>
       <c r="H49" s="63"/>
-      <c r="I49" s="149"/>
+      <c r="I49" s="181"/>
       <c r="K49" t="str">
         <f t="shared" si="6"/>
         <v>VEL-DT-NC-4</v>
@@ -2903,8 +2946,8 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="165"/>
-      <c r="B50" s="163"/>
+      <c r="A50" s="164"/>
+      <c r="B50" s="179"/>
       <c r="C50" s="61" t="s">
         <v>94</v>
       </c>
@@ -2920,7 +2963,7 @@
       </c>
       <c r="G50" s="64"/>
       <c r="H50" s="63"/>
-      <c r="I50" s="149"/>
+      <c r="I50" s="181"/>
       <c r="K50" t="str">
         <f t="shared" si="6"/>
         <v>VEL-DT-NC-5</v>
@@ -2930,8 +2973,8 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="165"/>
-      <c r="B51" s="163"/>
+      <c r="A51" s="164"/>
+      <c r="B51" s="179"/>
       <c r="C51" s="61" t="s">
         <v>95</v>
       </c>
@@ -2942,7 +2985,7 @@
       <c r="F51" s="63"/>
       <c r="G51" s="64"/>
       <c r="H51" s="63"/>
-      <c r="I51" s="149"/>
+      <c r="I51" s="181"/>
       <c r="K51" t="str">
         <f t="shared" si="6"/>
         <v>VEL-DT-NC-6</v>
@@ -2952,7 +2995,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="165"/>
+      <c r="A52" s="164"/>
       <c r="B52" s="120" t="s">
         <v>102</v>
       </c>
@@ -2978,8 +3021,8 @@
       </c>
     </row>
     <row r="53" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="165"/>
-      <c r="B53" s="167" t="s">
+      <c r="A53" s="164"/>
+      <c r="B53" s="166" t="s">
         <v>136</v>
       </c>
       <c r="C53" s="66" t="s">
@@ -2996,7 +3039,7 @@
       </c>
       <c r="G53" s="68"/>
       <c r="H53" s="67"/>
-      <c r="I53" s="150" t="s">
+      <c r="I53" s="182" t="s">
         <v>48</v>
       </c>
       <c r="K53" t="str">
@@ -3008,8 +3051,8 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="165"/>
-      <c r="B54" s="167"/>
+      <c r="A54" s="164"/>
+      <c r="B54" s="166"/>
       <c r="C54" s="66" t="s">
         <v>97</v>
       </c>
@@ -3024,7 +3067,7 @@
       </c>
       <c r="G54" s="68"/>
       <c r="H54" s="67"/>
-      <c r="I54" s="150"/>
+      <c r="I54" s="182"/>
       <c r="K54" t="str">
         <f t="shared" si="6"/>
         <v>VEL-CLNT-NC-2</v>
@@ -3034,8 +3077,8 @@
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="165"/>
-      <c r="B55" s="167"/>
+      <c r="A55" s="164"/>
+      <c r="B55" s="166"/>
       <c r="C55" s="66" t="s">
         <v>98</v>
       </c>
@@ -3050,7 +3093,7 @@
       </c>
       <c r="G55" s="68"/>
       <c r="H55" s="67"/>
-      <c r="I55" s="150"/>
+      <c r="I55" s="182"/>
       <c r="K55" t="str">
         <f t="shared" si="6"/>
         <v>VEL-CLNT-NC-3</v>
@@ -3060,8 +3103,8 @@
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="165"/>
-      <c r="B56" s="167"/>
+      <c r="A56" s="164"/>
+      <c r="B56" s="166"/>
       <c r="C56" s="66" t="s">
         <v>99</v>
       </c>
@@ -3076,7 +3119,7 @@
       </c>
       <c r="G56" s="68"/>
       <c r="H56" s="67"/>
-      <c r="I56" s="150"/>
+      <c r="I56" s="182"/>
       <c r="K56" t="str">
         <f t="shared" si="6"/>
         <v>VEL-CLNT-NC-4</v>
@@ -3086,8 +3129,8 @@
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="165"/>
-      <c r="B57" s="167"/>
+      <c r="A57" s="164"/>
+      <c r="B57" s="166"/>
       <c r="C57" s="66" t="s">
         <v>100</v>
       </c>
@@ -3103,7 +3146,7 @@
       </c>
       <c r="G57" s="68"/>
       <c r="H57" s="67"/>
-      <c r="I57" s="150"/>
+      <c r="I57" s="182"/>
       <c r="K57" t="str">
         <f t="shared" si="6"/>
         <v>VEL-CLNT-NC-5</v>
@@ -3113,7 +3156,7 @@
       </c>
     </row>
     <row r="58" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="165"/>
+      <c r="A58" s="164"/>
       <c r="B58" s="125" t="s">
         <v>102</v>
       </c>
@@ -3139,8 +3182,8 @@
       </c>
     </row>
     <row r="59" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="165"/>
-      <c r="B59" s="168" t="s">
+      <c r="A59" s="164"/>
+      <c r="B59" s="167" t="s">
         <v>78</v>
       </c>
       <c r="C59" s="69" t="s">
@@ -3157,7 +3200,7 @@
       </c>
       <c r="G59" s="72"/>
       <c r="H59" s="71"/>
-      <c r="I59" s="151" t="s">
+      <c r="I59" s="183" t="s">
         <v>48</v>
       </c>
       <c r="K59" t="str">
@@ -3169,8 +3212,8 @@
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="165"/>
-      <c r="B60" s="168"/>
+      <c r="A60" s="164"/>
+      <c r="B60" s="167"/>
       <c r="C60" s="69" t="s">
         <v>80</v>
       </c>
@@ -3185,7 +3228,7 @@
       </c>
       <c r="G60" s="72"/>
       <c r="H60" s="71"/>
-      <c r="I60" s="151"/>
+      <c r="I60" s="183"/>
       <c r="K60" t="str">
         <f t="shared" si="6"/>
         <v>VEL-DT-PURE-2</v>
@@ -3195,8 +3238,8 @@
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="165"/>
-      <c r="B61" s="168"/>
+      <c r="A61" s="164"/>
+      <c r="B61" s="167"/>
       <c r="C61" s="69" t="s">
         <v>81</v>
       </c>
@@ -3211,7 +3254,7 @@
       </c>
       <c r="G61" s="72"/>
       <c r="H61" s="71"/>
-      <c r="I61" s="151"/>
+      <c r="I61" s="183"/>
       <c r="K61" t="str">
         <f t="shared" si="6"/>
         <v>VEL-DT-PURE-3</v>
@@ -3221,8 +3264,8 @@
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="165"/>
-      <c r="B62" s="168"/>
+      <c r="A62" s="164"/>
+      <c r="B62" s="167"/>
       <c r="C62" s="69" t="s">
         <v>82</v>
       </c>
@@ -3237,7 +3280,7 @@
       </c>
       <c r="G62" s="72"/>
       <c r="H62" s="71"/>
-      <c r="I62" s="151"/>
+      <c r="I62" s="183"/>
       <c r="K62" t="str">
         <f t="shared" si="6"/>
         <v>VEL-DT-PURE-4</v>
@@ -3247,8 +3290,8 @@
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="165"/>
-      <c r="B63" s="168"/>
+      <c r="A63" s="164"/>
+      <c r="B63" s="167"/>
       <c r="C63" s="69" t="s">
         <v>83</v>
       </c>
@@ -3264,7 +3307,7 @@
       </c>
       <c r="G63" s="72"/>
       <c r="H63" s="71"/>
-      <c r="I63" s="151"/>
+      <c r="I63" s="183"/>
       <c r="J63" s="4"/>
       <c r="K63" t="str">
         <f t="shared" si="6"/>
@@ -3276,8 +3319,8 @@
       <c r="N63" s="20"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="165"/>
-      <c r="B64" s="168"/>
+      <c r="A64" s="164"/>
+      <c r="B64" s="167"/>
       <c r="C64" s="69" t="s">
         <v>84</v>
       </c>
@@ -3288,7 +3331,7 @@
       <c r="F64" s="71"/>
       <c r="G64" s="72"/>
       <c r="H64" s="71"/>
-      <c r="I64" s="151"/>
+      <c r="I64" s="183"/>
       <c r="K64" t="str">
         <f t="shared" si="6"/>
         <v>VEL-DT-PURE-6</v>
@@ -3300,7 +3343,7 @@
       <c r="N64" s="20"/>
     </row>
     <row r="65" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="165"/>
+      <c r="A65" s="164"/>
       <c r="B65" s="131" t="s">
         <v>102</v>
       </c>
@@ -3326,8 +3369,8 @@
       </c>
     </row>
     <row r="66" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="165"/>
-      <c r="B66" s="169" t="s">
+      <c r="A66" s="164"/>
+      <c r="B66" s="168" t="s">
         <v>137</v>
       </c>
       <c r="C66" s="74" t="s">
@@ -3344,7 +3387,7 @@
       </c>
       <c r="G66" s="76"/>
       <c r="H66" s="75"/>
-      <c r="I66" s="152" t="s">
+      <c r="I66" s="184" t="s">
         <v>48</v>
       </c>
       <c r="K66" t="str">
@@ -3356,8 +3399,8 @@
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="165"/>
-      <c r="B67" s="169"/>
+      <c r="A67" s="164"/>
+      <c r="B67" s="168"/>
       <c r="C67" s="74" t="s">
         <v>86</v>
       </c>
@@ -3372,7 +3415,7 @@
       </c>
       <c r="G67" s="76"/>
       <c r="H67" s="75"/>
-      <c r="I67" s="152"/>
+      <c r="I67" s="184"/>
       <c r="K67" t="str">
         <f t="shared" si="6"/>
         <v>VEL-CLNT-PURE-2</v>
@@ -3382,8 +3425,8 @@
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="165"/>
-      <c r="B68" s="169"/>
+      <c r="A68" s="164"/>
+      <c r="B68" s="168"/>
       <c r="C68" s="74" t="s">
         <v>87</v>
       </c>
@@ -3398,7 +3441,7 @@
       </c>
       <c r="G68" s="76"/>
       <c r="H68" s="75"/>
-      <c r="I68" s="152"/>
+      <c r="I68" s="184"/>
       <c r="K68" t="str">
         <f t="shared" si="6"/>
         <v>VEL-CLNT-PURE-3</v>
@@ -3408,8 +3451,8 @@
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="165"/>
-      <c r="B69" s="169"/>
+      <c r="A69" s="164"/>
+      <c r="B69" s="168"/>
       <c r="C69" s="74" t="s">
         <v>88</v>
       </c>
@@ -3424,7 +3467,7 @@
       </c>
       <c r="G69" s="76"/>
       <c r="H69" s="75"/>
-      <c r="I69" s="152"/>
+      <c r="I69" s="184"/>
       <c r="K69" t="str">
         <f t="shared" si="6"/>
         <v>VEL-CLNT-PURE-4</v>
@@ -3434,8 +3477,8 @@
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="166"/>
-      <c r="B70" s="170"/>
+      <c r="A70" s="165"/>
+      <c r="B70" s="169"/>
       <c r="C70" s="77" t="s">
         <v>89</v>
       </c>
@@ -3451,7 +3494,7 @@
       </c>
       <c r="G70" s="79"/>
       <c r="H70" s="78"/>
-      <c r="I70" s="153"/>
+      <c r="I70" s="185"/>
       <c r="K70" t="str">
         <f t="shared" ref="K70" si="7">C70</f>
         <v>VEL-CLNT-PURE-5</v>
@@ -3489,15 +3532,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="A27:A44"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A5:A20"/>
-    <mergeCell ref="B14:B20"/>
-    <mergeCell ref="B6:B12"/>
-    <mergeCell ref="I6:I12"/>
-    <mergeCell ref="I14:I20"/>
+    <mergeCell ref="I46:I51"/>
+    <mergeCell ref="I53:I57"/>
+    <mergeCell ref="I59:I64"/>
+    <mergeCell ref="I66:I70"/>
+    <mergeCell ref="I40:I44"/>
     <mergeCell ref="A45:A70"/>
     <mergeCell ref="B53:B57"/>
     <mergeCell ref="B59:B64"/>
@@ -3508,12 +3547,16 @@
     <mergeCell ref="B34:B38"/>
     <mergeCell ref="B40:B44"/>
     <mergeCell ref="B46:B51"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="A27:A44"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A5:A20"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="I6:I12"/>
+    <mergeCell ref="I14:I20"/>
     <mergeCell ref="I28:I32"/>
-    <mergeCell ref="I46:I51"/>
-    <mergeCell ref="I53:I57"/>
-    <mergeCell ref="I59:I64"/>
-    <mergeCell ref="I66:I70"/>
-    <mergeCell ref="I40:I44"/>
     <mergeCell ref="I34:I38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3522,7 +3565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4473,7 +4516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6085,7 +6128,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>